<commit_message>
privilige solved staff page not loading
</commit_message>
<xml_diff>
--- a/data/receptionists.xlsx
+++ b/data/receptionists.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,6 +561,73 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>maryam</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Maryam</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Maryam</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>923432928333</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Islamabad</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-02-25</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>250000</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>members,member_attendance,staff_attendance,payments,reports,staff,sales,inventory,packages</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>manager</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
staff navbar sync with the staff dashboard
</commit_message>
<xml_diff>
--- a/data/receptionists.xlsx
+++ b/data/receptionists.xlsx
@@ -516,8 +516,10 @@
           <t>Qasim</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>923432928333</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>923432928333</t>
+        </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -529,16 +531,20 @@
           <t>2025-03-07</t>
         </is>
       </c>
-      <c r="G2" t="n">
-        <v>20</v>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="I2" t="n">
-        <v>250000</v>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>250000</t>
+        </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -552,7 +558,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>members,attendance,payments,packages</t>
+          <t>members,staff_attendance,payments,packages</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -577,10 +583,8 @@
           <t>Maryam</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>923432928333</t>
-        </is>
+      <c r="D3" t="n">
+        <v>923432928333</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -592,20 +596,16 @@
           <t>2025-02-25</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="G3" t="n">
+        <v>20</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>250000</t>
-        </is>
+      <c r="I3" t="n">
+        <v>250000</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>

</xml_diff>